<commit_message>
Corrige typo na planilha, adiciona espaços, atualiza imagem
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -40,7 +40,7 @@
     <t>gratuito</t>
   </si>
   <si>
-    <t>"Soul For Us","Magic Circus","Diamond Power","Thang Of Thunder"</t>
+    <t>"Soul For Us", "Magic Circus", "Diamond Power", "Thang Of Thunder"</t>
   </si>
   <si>
     <t>Walter Phoenix, Freedie Shannon, Lance Day</t>
@@ -49,10 +49,10 @@
     <t>Cintia</t>
   </si>
   <si>
-    <t>famíliar</t>
-  </si>
-  <si>
-    <t>"Home Forever", "Words Of Her Life", "Reflections Of Magic", "Honey,Let's Be Silly"</t>
+    <t>familiar</t>
+  </si>
+  <si>
+    <t>"Home Forever", "Words Of Her Life", "Reflections Of Magic", "Honey, Let's Be Silly"</t>
   </si>
   <si>
     <t>Walter Phoenix, Lance Day</t>
@@ -73,7 +73,7 @@
     <t>Roger</t>
   </si>
   <si>
-    <t>"Dance With Her Own","Without My Streets", "Celebration Of More"</t>
+    <t>"Dance With Her Own", "Without My Streets", "Celebration Of More"</t>
   </si>
   <si>
     <t>Freedie Shannon</t>
@@ -97,13 +97,13 @@
     <t>Walter Phoenix</t>
   </si>
   <si>
-    <t>"Soul For Us","Reflections Of Magic","Dance With Her Own"</t>
+    <t>"Soul For Us", "Reflections Of Magic", "Dance With Her Own"</t>
   </si>
   <si>
     <t>Exuberant</t>
   </si>
   <si>
-    <t>"Troubles Of My Inner Fire”, “Time Fireworks”</t>
+    <t>"Troubles Of My Inner Fire", "Time Fireworks"</t>
   </si>
   <si>
     <t>Hallowed Steam</t>
@@ -112,7 +112,7 @@
     <t>Peter Strong</t>
   </si>
   <si>
-    <t>"Magic Circus", “Honey, So Do I", “Sweetie, Let’s Go Wild”, “She Knows”</t>
+    <t>"Magic Circus", "Honey, So Do I", "Sweetie, Let's Go Wild", "She Knows"</t>
   </si>
   <si>
     <t>Incandescent</t>
@@ -121,13 +121,13 @@
     <t>Lance Day</t>
   </si>
   <si>
-    <t>“Fantasy For Me”, "Celebration Of More”, "Rock His Everything”, "Home Forever”, "Diamond Power”, "Honey,Let's Be Silly”</t>
+    <t>"Fantasy For Me", "Celebration Of More", "Rock His Everything", "Home Forever", "Diamond Power", "Honey, Let's Be Silly"</t>
   </si>
   <si>
     <t>Temporary Culture</t>
   </si>
   <si>
-    <t>"Thang Of Thunder", “Words Of Her Life", “Without My Streets”</t>
+    <t>"Thang Of Thunder", "Words Of Her Life", "Without My Streets"</t>
   </si>
 </sst>
 </file>
@@ -156,7 +156,7 @@
     <font>
       <b val="1"/>
       <sz val="11"/>
-      <color indexed="10"/>
+      <color indexed="9"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -175,18 +175,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -196,51 +196,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="11"/>
       </left>
       <right/>
@@ -282,10 +237,10 @@
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -309,7 +264,7 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
@@ -321,10 +276,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
@@ -336,7 +291,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -354,41 +309,56 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -398,95 +368,89 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -506,10 +470,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff4472c4"/>
+      <rgbColor rgb="ff8eaadb"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff8eaadb"/>
-      <rgbColor rgb="ff4472c4"/>
       <rgbColor rgb="ffd9e2f3"/>
     </indexedColors>
   </colors>
@@ -1572,404 +1536,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="3.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.4688" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1406" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="38.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.3516" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="24" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.4688" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6719" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1406" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.3516" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="24" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+    <row r="1" ht="31.5" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" t="s" s="4">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s" s="10">
+        <v>9</v>
+      </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s" s="12">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" ht="31.5" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s" s="7">
+    <row r="3" ht="45" customHeight="1">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="14">
+        <v>11</v>
+      </c>
+      <c r="C3" s="15">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E3" s="15">
+        <v>7.99</v>
+      </c>
+      <c r="F3" t="s" s="16">
+        <v>13</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="31.5" customHeight="1">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="8">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5.99</v>
+      </c>
+      <c r="F4" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" ht="39" customHeight="1">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="14">
+        <v>19</v>
+      </c>
+      <c r="C5" s="15">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15">
         <v>0</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="F5" t="s" s="16">
+        <v>20</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s" s="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" ht="38.1" customHeight="1">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s" s="3">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s" s="3">
+        <v>25</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+    </row>
+    <row r="8" ht="26.55" customHeight="1">
+      <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="D3" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s" s="8">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s" s="8">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s" s="9">
-        <v>5</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" t="s" s="9">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s" s="11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s" s="13">
-        <v>7</v>
-      </c>
-      <c r="D4" s="14">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s" s="13">
-        <v>8</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s" s="17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" ht="45" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="18">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="D5" s="20">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s" s="19">
-        <v>12</v>
-      </c>
-      <c r="F5" s="20">
-        <v>7.99</v>
-      </c>
-      <c r="G5" t="s" s="21">
-        <v>13</v>
-      </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s" s="24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" ht="31.5" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="12">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s" s="13">
-        <v>15</v>
-      </c>
-      <c r="D6" s="14">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s" s="13">
-        <v>16</v>
-      </c>
-      <c r="F6" s="14">
-        <v>5.99</v>
-      </c>
-      <c r="G6" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="16">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s" s="17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" ht="39" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="18">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s" s="19">
-        <v>19</v>
-      </c>
-      <c r="D7" s="20">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s" s="19">
-        <v>8</v>
-      </c>
-      <c r="F7" s="20">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s" s="21">
-        <v>20</v>
-      </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s" s="24">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
+      <c r="B8" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="26">
+        <v>28</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="A9" s="13">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s" s="14">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s" s="27">
+        <v>30</v>
+      </c>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
-    <row r="10" ht="38.1" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+    <row r="10" ht="26.55" customHeight="1">
+      <c r="A10" s="7">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s" s="26">
+        <v>33</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" t="s" s="7">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s" s="8">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+    <row r="11" ht="39.55" customHeight="1">
+      <c r="A11" s="13">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s" s="14">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s" s="14">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s" s="27">
+        <v>36</v>
+      </c>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" ht="26.55" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="13">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="E12" t="s" s="28">
-        <v>28</v>
-      </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="18">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s" s="19">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s" s="19">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s" s="29">
-        <v>30</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" ht="26.55" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="12">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s" s="13">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s" s="28">
-        <v>33</v>
-      </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" ht="39.55" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="18">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s" s="19">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s" s="19">
-        <v>35</v>
-      </c>
-      <c r="E15" t="s" s="29">
-        <v>36</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" ht="26.55" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="12">
+      <c r="A12" s="7">
         <v>5</v>
       </c>
-      <c r="C16" t="s" s="13">
+      <c r="B12" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="D16" t="s" s="13">
+      <c r="C12" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="E16" t="s" s="28">
+      <c r="D12" t="s" s="26">
         <v>38</v>
       </c>
-      <c r="F16" s="27"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" ht="13.55" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" ht="13.55" customHeight="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>